<commit_message>
BillTo & Coordinates PDF - classes added
</commit_message>
<xml_diff>
--- a/InmarsatPDFExcel.xlsx
+++ b/InmarsatPDFExcel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>PDF File name</t>
   </si>
@@ -40,46 +40,12 @@
   </si>
   <si>
     <t>C:\Users\Trishita.Tadala\Desktop\IMS\XMLs\117976_986021_1386249_20190430.xml</t>
-  </si>
-  <si>
-    <t>C:\Users\Trishita.Tadala\Desktop\IMS\XMLs\118002_953973_1386301_20190430.xml</t>
-  </si>
-  <si>
-    <t>C:\Users\Trishita.Tadala\Desktop\IMS\Invoice\INVOICE_1386301_953973_201904.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Trishita.Tadala\Desktop\IMS\XMLs\118006_946415_1386305_20190430.xml</t>
-  </si>
-  <si>
-    <t>C:\Users\Trishita.Tadala\Desktop\IMS\Invoice\INVOICE_1386305_946415_201904.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Trishita.Tadala\Desktop\IMS\XMLs\118007_1037754_1386306_20190430.xml</t>
-  </si>
-  <si>
-    <t>C:\Users\Trishita.Tadala\Desktop\IMS\Invoice\INVOICE_1386306_1037754_201904.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Trishita.Tadala\Desktop\IMS\Invoice\INVOICE_1588207_946713_202002.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Trishita.Tadala\Desktop\IMS\XMLs\119618_946713_1588207_20200229.xml</t>
-  </si>
-  <si>
-    <t>C:\Users\Trishita.Tadala\Desktop\IMS\XMLs\10000601_114251_1588607_20200220.xml</t>
-  </si>
-  <si>
-    <t>C:\Users\Trishita.Tadala\Desktop\IMS\Invoice\CNT_9000001504192_114251_202002.pdf</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,7 +382,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -424,19 +390,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="82.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="55.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="22.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="43.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="3" width="27.42578125" collapsed="true"/>
+    <col min="1" max="1" width="65.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="51.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -463,83 +429,9 @@
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>